<commit_message>
Test Change,delete and multiple Sheets
</commit_message>
<xml_diff>
--- a/Mapping Test.xlsx
+++ b/Mapping Test.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://azyrasystemsltd-my.sharepoint.com/personal/cheryl_dunn_azyra_com/Documents/Documents/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{161EBA7E-DD53-41C4-89DC-00E2627D8C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C5507F9-2F07-46FB-908B-9C6A532BA3F0}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{161EBA7E-DD53-41C4-89DC-00E2627D8C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{184D1A3E-D98D-4A98-8210-D4DE2EB023B0}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DB461C79-30A9-4FD2-8B85-41A7E31CDED5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DB461C79-30A9-4FD2-8B85-41A7E31CDED5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ProcessResponse" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
   <si>
     <t>Updated By</t>
   </si>
@@ -83,12 +84,6 @@
     <t>Example Input</t>
   </si>
   <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>EDIFACT</t>
-  </si>
-  <si>
     <t>FillUpdate</t>
   </si>
   <si>
@@ -99,6 +94,24 @@
   </si>
   <si>
     <t>Error</t>
+  </si>
+  <si>
+    <t>ErrorTest123</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Property:Test</t>
+  </si>
+  <si>
+    <t>Test123</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Finished!</t>
   </si>
 </sst>
 </file>
@@ -479,11 +492,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C23BBA-C0F0-4ED8-8659-33A70C32457A}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -532,37 +562,154 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="4"/>
       <c r="F2" t="s">
         <v>15</v>
       </c>
       <c r="H2" t="s">
         <v>16</v>
       </c>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2"/>
+      <c r="Q2" s="5"/>
+      <c r="S2"/>
     </row>
     <row r="3" spans="1:19" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3"/>
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
       <c r="J3"/>
       <c r="K3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s">
         <v>19</v>
       </c>
-      <c r="M3" t="s">
+      <c r="P3"/>
+      <c r="Q3" s="5"/>
+      <c r="S3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795992CC-57F9-4202-984C-FA3F5618F4A7}">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="26.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="4"/>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2"/>
+      <c r="Q2" s="5"/>
+      <c r="S2"/>
+    </row>
+    <row r="3" spans="1:19" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="4"/>
+      <c r="F3" t="s">
         <v>20</v>
       </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3"/>
+      <c r="K3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3"/>
       <c r="P3"/>
-      <c r="Q3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="S3" t="s">
-        <v>20</v>
-      </c>
+      <c r="Q3" s="5"/>
+      <c r="S3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Testing XL Trail on a new branch
</commit_message>
<xml_diff>
--- a/Mapping Test.xlsx
+++ b/Mapping Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://azyrasystemsltd-my.sharepoint.com/personal/cheryl_dunn_azyra_com/Documents/Documents/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{161EBA7E-DD53-41C4-89DC-00E2627D8C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{184D1A3E-D98D-4A98-8210-D4DE2EB023B0}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{161EBA7E-DD53-41C4-89DC-00E2627D8C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D2CB933-D9D0-493B-922A-95661E52A42D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DB461C79-30A9-4FD2-8B85-41A7E31CDED5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DB461C79-30A9-4FD2-8B85-41A7E31CDED5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>Updated By</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>Finished!</t>
+  </si>
+  <si>
+    <t>Property:Test2</t>
+  </si>
+  <si>
+    <t>SQLTEXT</t>
+  </si>
+  <si>
+    <t>Test2342342</t>
   </si>
 </sst>
 </file>
@@ -490,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C23BBA-C0F0-4ED8-8659-33A70C32457A}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,6 +613,26 @@
       <c r="Q3" s="5"/>
       <c r="S3"/>
     </row>
+    <row r="4" spans="1:19" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4"/>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4"/>
+      <c r="K4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4"/>
+      <c r="P4"/>
+      <c r="Q4" s="5"/>
+      <c r="S4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -613,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795992CC-57F9-4202-984C-FA3F5618F4A7}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>